<commit_message>
LOI update and context + type for all
</commit_message>
<xml_diff>
--- a/results/artaxata/data/tga_AA.xlsx
+++ b/results/artaxata/data/tga_AA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Uine\Documents\R\MB\results\artaxata\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16615BC6-CBD3-4494-B77B-0DFD6393743D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD26F9B4-4408-4E60-A759-CCD57B2959D8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10155" yWindow="0" windowWidth="17715" windowHeight="15495" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="705" windowWidth="17715" windowHeight="15495" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TGA701-Table" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="80">
   <si>
     <t>Name</t>
   </si>
@@ -233,6 +233,33 @@
   </si>
   <si>
     <t>Mass_950</t>
+  </si>
+  <si>
+    <t>context</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>Hill II</t>
+  </si>
+  <si>
+    <t>mudbrick</t>
+  </si>
+  <si>
+    <t>Urartian silo</t>
+  </si>
+  <si>
+    <t>Phase I</t>
+  </si>
+  <si>
+    <t>Phase II or III</t>
+  </si>
+  <si>
+    <t>Phase II</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -242,7 +269,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -376,6 +403,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -719,10 +752,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1078,19 +1113,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="7" width="9.140625" style="2"/>
+    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1112,8 +1148,14 @@
       <c r="G1" s="2" t="s">
         <v>70</v>
       </c>
+      <c r="H1" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>72</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -1135,8 +1177,14 @@
       <c r="G2" s="2" t="s">
         <v>26</v>
       </c>
+      <c r="H2" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>74</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -1158,8 +1206,14 @@
       <c r="G3" s="2" t="s">
         <v>30</v>
       </c>
+      <c r="H3" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>74</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -1181,8 +1235,14 @@
       <c r="G4" s="2" t="s">
         <v>34</v>
       </c>
+      <c r="H4" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>74</v>
+      </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -1204,8 +1264,14 @@
       <c r="G5" s="2" t="s">
         <v>38</v>
       </c>
+      <c r="H5" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>79</v>
+      </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -1227,8 +1293,14 @@
       <c r="G6" s="2" t="s">
         <v>40</v>
       </c>
+      <c r="H6" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>74</v>
+      </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
@@ -1250,8 +1322,14 @@
       <c r="G7" s="2" t="s">
         <v>44</v>
       </c>
+      <c r="H7" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>74</v>
+      </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
@@ -1273,8 +1351,14 @@
       <c r="G8" s="2" t="s">
         <v>47</v>
       </c>
+      <c r="H8" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>74</v>
+      </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -1296,8 +1380,14 @@
       <c r="G9" s="2" t="s">
         <v>51</v>
       </c>
+      <c r="H9" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>74</v>
+      </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
@@ -1319,8 +1409,14 @@
       <c r="G10" s="2" t="s">
         <v>55</v>
       </c>
+      <c r="H10" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>74</v>
+      </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
@@ -1342,8 +1438,14 @@
       <c r="G11" s="2" t="s">
         <v>58</v>
       </c>
+      <c r="H11" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>74</v>
+      </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>20</v>
       </c>
@@ -1365,8 +1467,14 @@
       <c r="G12" s="2" t="s">
         <v>62</v>
       </c>
+      <c r="H12" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>74</v>
+      </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>21</v>
       </c>
@@ -1387,6 +1495,12 @@
       </c>
       <c r="G13" s="2" t="s">
         <v>66</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>